<commit_message>
added rankings to the Q1 answer, the Jobs file
</commit_message>
<xml_diff>
--- a/assignment/Jobs.xlsx
+++ b/assignment/Jobs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavien M\Documents\University\Work\Foundations of ML\programming\assignment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4684936F-1D53-45F7-A835-ECF9C5CA133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,107 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+  <si>
+    <t>Job Name</t>
+  </si>
+  <si>
+    <t>Median Pay</t>
+  </si>
+  <si>
+    <t>Education Required</t>
+  </si>
+  <si>
+    <t>Number of Jobs</t>
+  </si>
+  <si>
+    <t>Future Employment Change</t>
+  </si>
+  <si>
+    <t>Future Job Outlook</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
+  </si>
+  <si>
+    <t>Software Developers</t>
+  </si>
+  <si>
+    <t>Information Security Analyst</t>
+  </si>
+  <si>
+    <t>Computer Network Architect</t>
+  </si>
+  <si>
+    <t>Database Administrator/Architect</t>
+  </si>
+  <si>
+    <t>Web Developer</t>
+  </si>
+  <si>
+    <t>16% </t>
+  </si>
+  <si>
+    <t>Computer and Information Research Scientists</t>
+  </si>
+  <si>
+    <t>Masters</t>
+  </si>
+  <si>
+    <t>Work Experience Required</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>&lt;5 yrs</t>
+  </si>
+  <si>
+    <t>&gt;5 yrs</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 2 aspects to jobs that I like: creating new things &amp; high pay. This job has both. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is similar to Software Dev, but it has higher entry requirements for little increase in pay, making it my second favorite job. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">While this job doesn't exactly create anything new, creating different computer networks for different purposes can be fund + it has high pay. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I like the problem solving aspect of cybersecurity, though it's not as innovative as other jobs, and it still has high pay. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Though it's not as innovative as other jobs, finding new patterns can be fun. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reason database is so low is because there are only so many ways to set up a databsase. While this job is high paying and crucial to the running of certain organizations, I would become bored rather quickly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This job ranks the lowest because it has the lowest pay and doesn't have a lot of innovation in its field. I don't count new fonts or UI as "innovation". A website is a website. </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +132,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,12 +168,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +506,282 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="33.109375" customWidth="1"/>
+    <col min="10" max="10" width="171.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9">
+        <v>103500</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="10">
+        <v>168900</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="H2" s="3">
+        <v>59400</v>
+      </c>
+      <c r="I2" s="12">
+        <v>5</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>124200</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1795300</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H3" s="3">
+        <v>451200</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>112000</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3">
+        <v>168900</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="H4" s="3">
+        <v>53200</v>
+      </c>
+      <c r="I4" s="12">
+        <v>4</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>126900</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
+        <v>180200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6300</v>
+      </c>
+      <c r="I5" s="12">
+        <v>3</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>112120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3">
+        <v>149300</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="H6" s="7">
+        <v>12300</v>
+      </c>
+      <c r="I6" s="12">
+        <v>6</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>80730</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3">
+        <v>216700</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3">
+        <v>34700</v>
+      </c>
+      <c r="I7" s="12">
+        <v>7</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5">
+        <v>136620</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3">
+        <v>36500</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8300</v>
+      </c>
+      <c r="I8" s="12">
+        <v>2</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did formatting for Q1 answer (Jobs Excel file)
</commit_message>
<xml_diff>
--- a/assignment/Jobs.xlsx
+++ b/assignment/Jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavien M\Documents\University\Work\Foundations of ML\programming\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4684936F-1D53-45F7-A835-ECF9C5CA133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320D1026-2F7E-46AA-AC6E-28F2760C9903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Job Name</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t xml:space="preserve">This job ranks the lowest because it has the lowest pay and doesn't have a lot of innovation in its field. I don't count new fonts or UI as "innovation". A website is a website. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavien's Note: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only thing that surprised me was that the Computer and Information Research Scientists did not require any previous work experience, despite the Masters requirement and the much higher pay. Other than that, everything was more or less what I expected. </t>
   </si>
 </sst>
 </file>
@@ -200,9 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -215,18 +221,16 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,34 +529,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -581,10 +585,10 @@
       <c r="H2" s="3">
         <v>59400</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="1">
         <v>5</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -613,10 +617,10 @@
       <c r="H3" s="3">
         <v>451200</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -645,10 +649,10 @@
       <c r="H4" s="3">
         <v>53200</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="1">
         <v>4</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -677,10 +681,10 @@
       <c r="H5" s="3">
         <v>6300</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="1">
         <v>3</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -709,10 +713,10 @@
       <c r="H6" s="7">
         <v>12300</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="1">
         <v>6</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -735,21 +739,21 @@
       <c r="F7" s="3">
         <v>216700</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="3">
         <v>34700</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="1">
         <v>7</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5">
@@ -773,11 +777,21 @@
       <c r="H8" s="3">
         <v>8300</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="1">
         <v>2</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>